<commit_message>
Have a working setup with that we need to template.
</commit_message>
<xml_diff>
--- a/Project_ErrorHandler/Project ErrorHandler.xlsx
+++ b/Project_ErrorHandler/Project ErrorHandler.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avhijfte/MulesoftProjects/Project_ErrorHandler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avhijfte/git/n-TGR/Project_ErrorHandler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8127E4A8-4B51-914C-8ACC-F944F5A4EC9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028D76FC-A804-5549-AAA8-F174B303FCAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31820" yWindow="2840" windowWidth="25040" windowHeight="14860" activeTab="1" xr2:uid="{4F3607DE-4CFA-1342-8748-2F6B2A7F18B6}"/>
+    <workbookView xWindow="-33000" yWindow="3440" windowWidth="25040" windowHeight="14860" activeTab="2" xr2:uid="{4F3607DE-4CFA-1342-8748-2F6B2A7F18B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Findings" sheetId="2" r:id="rId2"/>
+    <sheet name="Deployment" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Component and base url</t>
   </si>
@@ -281,13 +282,28 @@
   </si>
   <si>
     <t>This happens because the payload was no longer the way it is before you map it for storing in the database.</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>PROD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -338,8 +354,16 @@
       <name val="Monaco"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +373,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -398,6 +428,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,7 +896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DAED3C-8D68-7E46-9A08-E430F5CF8B34}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -896,4 +927,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDA248F-E989-924A-AD6D-BA94341A9BD6}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>